<commit_message>
Add semicolon to LCD generator output
</commit_message>
<xml_diff>
--- a/Keyestudio LCD Generator.xlsx
+++ b/Keyestudio LCD Generator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://barclays-my.sharepoint.com/personal/jonathan_hunter_barclays_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhunter/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7439E3A-E3BD-4709-9C1A-5D6A432CC904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CAEA27-CA5F-0A4A-9AA8-14F709CB96EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="24105" windowHeight="13830" xr2:uid="{6E856703-089C-4EB1-811A-12751249CB6E}"/>
+    <workbookView xWindow="1500" yWindow="700" windowWidth="24100" windowHeight="13840" xr2:uid="{6E856703-089C-4EB1-811A-12751249CB6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Generator" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="BinaryValues">Generator!$A$3:$A$9</definedName>
     <definedName name="EditArea">Generator!$B$3:$Q$9</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -646,15 +645,15 @@
   <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="17" width="3.7109375" customWidth="1"/>
+    <col min="2" max="17" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -681,7 +680,7 @@
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -706,7 +705,7 @@
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -741,7 +740,7 @@
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -776,7 +775,7 @@
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -811,7 +810,7 @@
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>8</v>
       </c>
@@ -846,7 +845,7 @@
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>16</v>
       </c>
@@ -881,7 +880,7 @@
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>32</v>
       </c>
@@ -916,7 +915,7 @@
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
     </row>
-    <row r="9" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>64</v>
       </c>
@@ -943,7 +942,7 @@
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="str">
         <f t="shared" ref="B10:P10" si="0">DEC2HEX(SUMIFS(BinaryValues,B3:B9,"x"),2)</f>
@@ -1016,7 +1015,7 @@
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1041,13 +1040,13 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:23" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="2" t="str">
-        <f>CONCATENATE("{0x",B10,",0x",C10,",0x",D10,",0x",E10,",0x",F10,",0x",G10,",0x",H10,",0x",I10,",0x",J10,",0x",K10,",0x",L10,",0x",M10,",0x",N10,",0x",O10,",0x",P10,",0x",Q10," }")</f>
-        <v>{0x00,0x3F,0x25,0x1A,0x00,0x00,0x00,0x00,0x00,0x00,0x00,0x00,0x3F,0x25,0x1A,0x00 }</v>
+        <f>CONCATENATE("{0x",B10,",0x",C10,",0x",D10,",0x",E10,",0x",F10,",0x",G10,",0x",H10,",0x",I10,",0x",J10,",0x",K10,",0x",L10,",0x",M10,",0x",N10,",0x",O10,",0x",P10,",0x",Q10," };")</f>
+        <v>{0x00,0x3F,0x25,0x1A,0x00,0x00,0x00,0x00,0x00,0x00,0x00,0x00,0x3F,0x25,0x1A,0x00 };</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1071,7 +1070,7 @@
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1096,7 +1095,7 @@
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1121,7 +1120,7 @@
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1146,7 +1145,7 @@
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1171,7 +1170,7 @@
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1196,7 +1195,7 @@
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1221,7 +1220,7 @@
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1246,7 +1245,7 @@
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1271,7 +1270,7 @@
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1296,7 +1295,7 @@
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1321,7 +1320,7 @@
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1346,7 +1345,7 @@
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1394,12 +1393,12 @@
       <selection activeCell="C2" sqref="C2:R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="18" width="3.85546875" customWidth="1"/>
+    <col min="3" max="18" width="3.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1424,7 +1423,7 @@
       <c r="Q2" s="7"/>
       <c r="R2" s="8"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C3" s="9"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -1450,7 +1449,7 @@
       <c r="Q3" s="10"/>
       <c r="R3" s="11"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -1476,7 +1475,7 @@
       <c r="Q4" s="10"/>
       <c r="R4" s="11"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -1502,7 +1501,7 @@
       <c r="Q5" s="10"/>
       <c r="R5" s="11"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -1532,7 +1531,7 @@
       <c r="Q6" s="10"/>
       <c r="R6" s="11"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
@@ -1566,7 +1565,7 @@
       <c r="Q7" s="10"/>
       <c r="R7" s="11"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C8" s="12"/>
       <c r="D8" s="13" t="s">
         <v>1</v>
@@ -1600,7 +1599,7 @@
       </c>
       <c r="R8" s="14"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1637,7 +1636,7 @@
       </c>
       <c r="R10" s="8"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10" t="s">
@@ -1671,7 +1670,7 @@
       <c r="Q11" s="10"/>
       <c r="R11" s="11"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -1701,7 +1700,7 @@
       <c r="Q12" s="10"/>
       <c r="R12" s="11"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -1727,7 +1726,7 @@
       <c r="Q13" s="10"/>
       <c r="R13" s="11"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -1753,7 +1752,7 @@
       <c r="Q14" s="10"/>
       <c r="R14" s="11"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -1779,7 +1778,7 @@
       <c r="Q15" s="10"/>
       <c r="R15" s="11"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C16" s="12"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
@@ -1801,7 +1800,7 @@
       <c r="Q16" s="13"/>
       <c r="R16" s="14"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1836,7 +1835,7 @@
       <c r="Q18" s="7"/>
       <c r="R18" s="8"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C19" s="9" t="s">
         <v>1</v>
       </c>
@@ -1870,7 +1869,7 @@
       <c r="Q19" s="10"/>
       <c r="R19" s="11"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C20" s="9"/>
       <c r="D20" s="10" t="s">
         <v>1</v>
@@ -1904,7 +1903,7 @@
       </c>
       <c r="R20" s="11"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10" t="s">
@@ -1938,7 +1937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C22" s="9"/>
       <c r="D22" s="10" t="s">
         <v>1</v>
@@ -1972,7 +1971,7 @@
       </c>
       <c r="R22" s="11"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C23" s="9" t="s">
         <v>1</v>
       </c>
@@ -2006,7 +2005,7 @@
       <c r="Q23" s="10"/>
       <c r="R23" s="11"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C24" s="12" t="s">
         <v>1</v>
       </c>
@@ -2038,7 +2037,7 @@
       <c r="Q24" s="13"/>
       <c r="R24" s="14"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -2073,7 +2072,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10" t="s">
@@ -2107,7 +2106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C28" s="9"/>
       <c r="D28" s="10" t="s">
         <v>7</v>
@@ -2141,7 +2140,7 @@
       </c>
       <c r="R28" s="11"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C29" s="9" t="s">
         <v>7</v>
       </c>
@@ -2175,7 +2174,7 @@
       <c r="Q29" s="10"/>
       <c r="R29" s="11"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C30" s="9"/>
       <c r="D30" s="10" t="s">
         <v>7</v>
@@ -2209,7 +2208,7 @@
       </c>
       <c r="R30" s="11"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C31" s="9"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10" t="s">
@@ -2243,7 +2242,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C32" s="12"/>
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
@@ -2275,7 +2274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -2300,7 +2299,7 @@
       <c r="Q34" s="7"/>
       <c r="R34" s="8"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C35" s="9"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
@@ -2332,7 +2331,7 @@
       <c r="Q35" s="10"/>
       <c r="R35" s="11"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C36" s="9"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10" t="s">
@@ -2374,7 +2373,7 @@
       <c r="Q36" s="10"/>
       <c r="R36" s="11"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C37" s="9"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
@@ -2412,7 +2411,7 @@
       <c r="Q37" s="10"/>
       <c r="R37" s="11"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C38" s="9"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
@@ -2446,7 +2445,7 @@
       <c r="Q38" s="10"/>
       <c r="R38" s="11"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C39" s="9"/>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
@@ -2476,7 +2475,7 @@
       <c r="Q39" s="10"/>
       <c r="R39" s="11"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C40" s="12"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>

</xml_diff>